<commit_message>
Working on generating oscillations.
Found my model’s result is not consistent with 2008 model by the first
trough.
</commit_message>
<xml_diff>
--- a/docs/parsTable.xlsx
+++ b/docs/parsTable.xlsx
@@ -1565,8 +1565,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="505">
+  <cellStyleXfs count="513">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2292,6 +2300,42 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2328,44 +2372,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="505">
+  <cellStyles count="513">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2618,6 +2626,10 @@
     <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2870,6 +2882,10 @@
     <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3328,9 +3344,10 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{9DBE73BB-A8CF-B84F-9AC0-F4F74DC9C616}" name="zhang Cheng" id="-845641123" dateTime="2014-03-14T11:27:26"/>
+  <userInfo guid="{9DBE73BB-A8CF-B84F-9AC0-F4F74DC9C616}" name="zhang Cheng" id="-845611106" dateTime="2014-05-14T16:58:41"/>
 </users>
 </file>
 
@@ -4726,8 +4743,8 @@
   </sheetPr>
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4743,51 +4760,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" ht="36" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="111" t="s">
+      <c r="D1" s="96"/>
+      <c r="E1" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="111" t="s">
+      <c r="F1" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="111" t="s">
+      <c r="G1" s="93" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="27"/>
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1">
-      <c r="A2" s="110"/>
-      <c r="B2" s="110"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
       <c r="C2" s="41" t="s">
         <v>265</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>266</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
     </row>
     <row r="3" spans="1:9" ht="40">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="103" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="93"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="105"/>
       <c r="H3" s="28"/>
       <c r="I3" s="29"/>
     </row>
@@ -5186,7 +5203,7 @@
       <c r="A21" s="58">
         <v>18</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="106" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="70"/>
@@ -5196,7 +5213,7 @@
       <c r="E21" s="71" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="97" t="s">
+      <c r="F21" s="109" t="s">
         <v>121</v>
       </c>
       <c r="G21" s="66" t="s">
@@ -5209,7 +5226,7 @@
       <c r="A22" s="30">
         <v>19</v>
       </c>
-      <c r="B22" s="95"/>
+      <c r="B22" s="107"/>
       <c r="C22" s="33"/>
       <c r="D22" s="15">
         <v>3</v>
@@ -5217,7 +5234,7 @@
       <c r="E22" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="98"/>
+      <c r="F22" s="110"/>
       <c r="G22" s="38" t="s">
         <v>196</v>
       </c>
@@ -5228,7 +5245,7 @@
       <c r="A23" s="58">
         <v>20</v>
       </c>
-      <c r="B23" s="96"/>
+      <c r="B23" s="108"/>
       <c r="C23" s="60"/>
       <c r="D23" s="60">
         <v>5.7936000000000001E-2</v>
@@ -5236,7 +5253,7 @@
       <c r="E23" s="71" t="s">
         <v>181</v>
       </c>
-      <c r="F23" s="99"/>
+      <c r="F23" s="111"/>
       <c r="G23" s="66" t="s">
         <v>189</v>
       </c>
@@ -5313,15 +5330,15 @@
       <c r="I26" s="29"/>
     </row>
     <row r="27" spans="1:9" ht="40">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="93"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="105"/>
       <c r="H27" s="48"/>
       <c r="I27" s="48" t="s">
         <v>273</v>
@@ -5595,15 +5612,15 @@
       <c r="I38" s="29"/>
     </row>
     <row r="39" spans="1:11" ht="40">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="93"/>
+      <c r="B39" s="104"/>
+      <c r="C39" s="104"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="104"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="105"/>
       <c r="H39" s="28"/>
       <c r="I39" s="29"/>
     </row>
@@ -5945,15 +5962,15 @@
       <c r="L53" s="53"/>
     </row>
     <row r="58" spans="1:12" ht="40">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="B58" s="101"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="101"/>
-      <c r="E58" s="101"/>
-      <c r="F58" s="101"/>
-      <c r="G58" s="102"/>
+      <c r="B58" s="113"/>
+      <c r="C58" s="113"/>
+      <c r="D58" s="113"/>
+      <c r="E58" s="113"/>
+      <c r="F58" s="113"/>
+      <c r="G58" s="114"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="23" t="s">
@@ -6046,7 +6063,7 @@
       <c r="A63" s="36">
         <v>4</v>
       </c>
-      <c r="B63" s="103" t="s">
+      <c r="B63" s="97" t="s">
         <v>204</v>
       </c>
       <c r="C63" s="15">
@@ -6058,7 +6075,7 @@
       <c r="E63" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="F63" s="106" t="s">
+      <c r="F63" s="100" t="s">
         <v>256</v>
       </c>
       <c r="G63" s="9" t="s">
@@ -6070,7 +6087,7 @@
       <c r="A64" s="36">
         <v>7</v>
       </c>
-      <c r="B64" s="104"/>
+      <c r="B64" s="98"/>
       <c r="C64" s="15">
         <v>3</v>
       </c>
@@ -6080,7 +6097,7 @@
       <c r="E64" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="F64" s="107"/>
+      <c r="F64" s="101"/>
       <c r="G64" s="9" t="s">
         <v>264</v>
       </c>
@@ -6090,7 +6107,7 @@
       <c r="A65" s="36">
         <v>10</v>
       </c>
-      <c r="B65" s="105"/>
+      <c r="B65" s="99"/>
       <c r="C65" s="15">
         <v>0</v>
       </c>
@@ -6100,7 +6117,7 @@
       <c r="E65" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="F65" s="108"/>
+      <c r="F65" s="102"/>
       <c r="G65" s="21" t="s">
         <v>264</v>
       </c>
@@ -6110,7 +6127,7 @@
       <c r="A66" s="36">
         <v>5</v>
       </c>
-      <c r="B66" s="103" t="s">
+      <c r="B66" s="97" t="s">
         <v>205</v>
       </c>
       <c r="C66" s="15">
@@ -6122,7 +6139,7 @@
       <c r="E66" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="F66" s="106" t="s">
+      <c r="F66" s="100" t="s">
         <v>256</v>
       </c>
       <c r="G66" s="21" t="s">
@@ -6134,7 +6151,7 @@
       <c r="A67" s="36">
         <v>8</v>
       </c>
-      <c r="B67" s="104"/>
+      <c r="B67" s="98"/>
       <c r="C67" s="15">
         <v>3</v>
       </c>
@@ -6144,7 +6161,7 @@
       <c r="E67" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="F67" s="107"/>
+      <c r="F67" s="101"/>
       <c r="G67" s="21" t="s">
         <v>264</v>
       </c>
@@ -6154,7 +6171,7 @@
       <c r="A68" s="36">
         <v>11</v>
       </c>
-      <c r="B68" s="105"/>
+      <c r="B68" s="99"/>
       <c r="C68" s="15">
         <v>37</v>
       </c>
@@ -6164,7 +6181,7 @@
       <c r="E68" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="F68" s="108"/>
+      <c r="F68" s="102"/>
       <c r="G68" s="21" t="s">
         <v>264</v>
       </c>
@@ -6174,7 +6191,7 @@
       <c r="A69" s="36">
         <v>6</v>
       </c>
-      <c r="B69" s="103" t="s">
+      <c r="B69" s="97" t="s">
         <v>209</v>
       </c>
       <c r="C69" s="15">
@@ -6186,7 +6203,7 @@
       <c r="E69" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="F69" s="106" t="s">
+      <c r="F69" s="100" t="s">
         <v>256</v>
       </c>
       <c r="G69" s="21" t="s">
@@ -6198,7 +6215,7 @@
       <c r="A70" s="36">
         <v>9</v>
       </c>
-      <c r="B70" s="104"/>
+      <c r="B70" s="98"/>
       <c r="C70" s="15">
         <v>3</v>
       </c>
@@ -6208,7 +6225,7 @@
       <c r="E70" s="38" t="s">
         <v>267</v>
       </c>
-      <c r="F70" s="107"/>
+      <c r="F70" s="101"/>
       <c r="G70" s="21" t="s">
         <v>264</v>
       </c>
@@ -6218,7 +6235,7 @@
       <c r="A71" s="36">
         <v>12</v>
       </c>
-      <c r="B71" s="105"/>
+      <c r="B71" s="99"/>
       <c r="C71" s="15">
         <v>37</v>
       </c>
@@ -6228,7 +6245,7 @@
       <c r="E71" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="F71" s="108"/>
+      <c r="F71" s="102"/>
       <c r="G71" s="21" t="s">
         <v>264</v>
       </c>
@@ -7429,24 +7446,24 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="18">
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="F63:F65"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="F69:F71"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="F63:F65"/>
-    <mergeCell ref="F66:F68"/>
-    <mergeCell ref="F69:F71"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>